<commit_message>
increase maximum role colunms in uploader to 12
</commit_message>
<xml_diff>
--- a/Utilities/QMXFGenerator/InformationModel.xlsx
+++ b/Utilities/QMXFGenerator/InformationModel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="23955" windowHeight="10035" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="23955" windowHeight="10035" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Class" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="88">
   <si>
     <t>Load</t>
   </si>
@@ -208,6 +208,81 @@
   </si>
   <si>
     <t>popoioiopo</t>
+  </si>
+  <si>
+    <t>Role8 ID</t>
+  </si>
+  <si>
+    <t>Role8 Name</t>
+  </si>
+  <si>
+    <t>Role8 Description</t>
+  </si>
+  <si>
+    <t>Role8 Type</t>
+  </si>
+  <si>
+    <t>Role8 Value</t>
+  </si>
+  <si>
+    <t>Role9 ID</t>
+  </si>
+  <si>
+    <t>Role9 Name</t>
+  </si>
+  <si>
+    <t>Role9 Description</t>
+  </si>
+  <si>
+    <t>Role9 Type</t>
+  </si>
+  <si>
+    <t>Role9 Value</t>
+  </si>
+  <si>
+    <t>Role10 ID</t>
+  </si>
+  <si>
+    <t>Role10 Name</t>
+  </si>
+  <si>
+    <t>Role10 Description</t>
+  </si>
+  <si>
+    <t>Role10 Type</t>
+  </si>
+  <si>
+    <t>Role10 Value</t>
+  </si>
+  <si>
+    <t>Role11 ID</t>
+  </si>
+  <si>
+    <t>Role11 Name</t>
+  </si>
+  <si>
+    <t>Role11 Description</t>
+  </si>
+  <si>
+    <t>Role11 Type</t>
+  </si>
+  <si>
+    <t>Role11 Value</t>
+  </si>
+  <si>
+    <t>Role12 ID</t>
+  </si>
+  <si>
+    <t>Role12 Name</t>
+  </si>
+  <si>
+    <t>Role12 Description</t>
+  </si>
+  <si>
+    <t>Role12 Type</t>
+  </si>
+  <si>
+    <t>Role12 Value</t>
   </si>
 </sst>
 </file>
@@ -748,10 +823,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AT2"/>
+  <dimension ref="A1:BX2"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" workbookViewId="0">
-      <selection sqref="A1:AT1"/>
+    <sheetView tabSelected="1" topLeftCell="BB1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:BY1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -802,7 +877,7 @@
     <col min="46" max="46" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="15.75" thickBot="1">
+    <row r="1" spans="1:76" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -941,8 +1016,98 @@
       <c r="AT1" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="AU1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BN1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BS1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BX1" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="2" spans="1:46" ht="15.75" thickTop="1"/>
+    <row r="2" spans="1:76" ht="15.75" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1162,10 +1327,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AT2"/>
+  <dimension ref="A1:BX2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="BL1" workbookViewId="0">
+      <selection activeCell="BX1" sqref="L1:BX1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1216,7 +1381,7 @@
     <col min="46" max="46" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="15.75" thickBot="1">
+    <row r="1" spans="1:76" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1355,8 +1520,98 @@
       <c r="AT1" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="AU1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BN1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BS1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BX1" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="2" spans="1:46" ht="15.75" thickTop="1"/>
+    <row r="2" spans="1:76" ht="15.75" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>